<commit_message>
Updates nursery and RGBHV cables
</commit_message>
<xml_diff>
--- a/data/cables.xlsx
+++ b/data/cables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AE59DA-1AB9-404F-88BB-BA9EB9A6D2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E28D8-72E3-0A4D-9832-5FDE6FAF7DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="165">
   <si>
     <t>Tag</t>
   </si>
@@ -529,12 +529,6 @@
   </si>
   <si>
     <t>2307-2320</t>
-  </si>
-  <si>
-    <t>Reserved for Cat cable to Nursery --- which may not exist</t>
-  </si>
-  <si>
-    <t>2307-xxxx</t>
   </si>
   <si>
     <t>RGBHV</t>
@@ -1879,10 +1873,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="340" zoomScaleNormal="340" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3288,7 +3282,7 @@
         <v>162</v>
       </c>
       <c r="F57" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="G57" t="s">
         <v>38</v>
@@ -3297,30 +3291,13 @@
         <v>107</v>
       </c>
       <c r="I57" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
         <v>164</v>
-      </c>
-      <c r="F58" t="s">
-        <v>165</v>
-      </c>
-      <c r="G58" t="s">
-        <v>38</v>
-      </c>
-      <c r="H58" t="s">
-        <v>107</v>
-      </c>
-      <c r="I58" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="65" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="57" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
updated with Youth and Main labels
</commit_message>
<xml_diff>
--- a/data/cables.xlsx
+++ b/data/cables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A037C9-E528-0C4B-A17F-CB08B3DFF2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2682FBC1-A839-E443-AFEC-9C3397339AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="-17180" windowWidth="50720" windowHeight="26740" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
+    <workbookView xWindow="-60780" yWindow="-22120" windowWidth="59780" windowHeight="31680" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="237">
   <si>
     <t>Tag</t>
   </si>
@@ -198,9 +198,6 @@
     <t>2307-1824</t>
   </si>
   <si>
-    <t>sdi/din</t>
-  </si>
-  <si>
     <t>short</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>2307-2300</t>
   </si>
   <si>
-    <t>hdmi out 6</t>
-  </si>
-  <si>
     <t>ZVIU-B001</t>
   </si>
   <si>
@@ -573,39 +567,15 @@
     <t>DstPort</t>
   </si>
   <si>
-    <t>HDbTa</t>
-  </si>
-  <si>
-    <t>HDbTb</t>
-  </si>
-  <si>
-    <t>HDbTc</t>
-  </si>
-  <si>
-    <t>HDbTd</t>
-  </si>
-  <si>
-    <t>HDbTe</t>
-  </si>
-  <si>
-    <t>HDbTf</t>
-  </si>
-  <si>
     <t>2308-0800</t>
   </si>
   <si>
     <t>aux</t>
   </si>
   <si>
-    <t>2308-0804</t>
-  </si>
-  <si>
     <t>HdmiOut</t>
   </si>
   <si>
-    <t>2308-0803</t>
-  </si>
-  <si>
     <t>InputD</t>
   </si>
   <si>
@@ -615,21 +585,12 @@
     <t>Optical Hdmi</t>
   </si>
   <si>
-    <t>2308-0802</t>
-  </si>
-  <si>
-    <t>2308-0805</t>
-  </si>
-  <si>
     <t>InputC</t>
   </si>
   <si>
     <t>For guest on-stage</t>
   </si>
   <si>
-    <t>2308-0806</t>
-  </si>
-  <si>
     <t>CDWU-A002</t>
   </si>
   <si>
@@ -639,9 +600,6 @@
     <t>Video card HDMI Output</t>
   </si>
   <si>
-    <t>2308-0807</t>
-  </si>
-  <si>
     <t>RearGuest</t>
   </si>
   <si>
@@ -651,21 +609,12 @@
     <t>In1</t>
   </si>
   <si>
-    <t>2308-0809</t>
-  </si>
-  <si>
     <t>VMNU-0029</t>
   </si>
   <si>
     <t>vga</t>
   </si>
   <si>
-    <t>2308-0810</t>
-  </si>
-  <si>
-    <t>2308-0808</t>
-  </si>
-  <si>
     <t>quad3_sdi5</t>
   </si>
   <si>
@@ -699,9 +648,6 @@
     <t>hdmi_dongle</t>
   </si>
   <si>
-    <t>2308-0811</t>
-  </si>
-  <si>
     <t>Mic_In</t>
   </si>
   <si>
@@ -709,6 +655,102 @@
   </si>
   <si>
     <t>rack_dev</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>2308-0915</t>
+  </si>
+  <si>
+    <t>2308-0916</t>
+  </si>
+  <si>
+    <t>2308-0917</t>
+  </si>
+  <si>
+    <t>2308-0918</t>
+  </si>
+  <si>
+    <t>2308-0919</t>
+  </si>
+  <si>
+    <t>out_1_HDbT</t>
+  </si>
+  <si>
+    <t>out_2_HDbT</t>
+  </si>
+  <si>
+    <t>out_3_HDbT</t>
+  </si>
+  <si>
+    <t>out_4_HDbT</t>
+  </si>
+  <si>
+    <t>hdmi_out</t>
+  </si>
+  <si>
+    <t>PROJ0001</t>
+  </si>
+  <si>
+    <t>PROJ0002</t>
+  </si>
+  <si>
+    <t>PROJ0003</t>
+  </si>
+  <si>
+    <t>cat6e</t>
+  </si>
+  <si>
+    <t>out_7_HDbT</t>
+  </si>
+  <si>
+    <t>out_8_HDbT</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>out_5_hdmi</t>
+  </si>
+  <si>
+    <t>2308-0920</t>
+  </si>
+  <si>
+    <t>kramer</t>
+  </si>
+  <si>
+    <t>2308-0004</t>
+  </si>
+  <si>
+    <t>2308-0005</t>
+  </si>
+  <si>
+    <t>2308-0006</t>
+  </si>
+  <si>
+    <t>2308-0007</t>
+  </si>
+  <si>
+    <t>2308-0009</t>
+  </si>
+  <si>
+    <t>2308-0010</t>
+  </si>
+  <si>
+    <t>2308-0011</t>
+  </si>
+  <si>
+    <t>2308-0008</t>
+  </si>
+  <si>
+    <t>2308-0002</t>
+  </si>
+  <si>
+    <t>2308-0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optical </t>
   </si>
 </sst>
 </file>
@@ -819,42 +861,46 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45130.595223379627" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="57" xr:uid="{29F59781-2A20-324D-894E-ECA5B1C78DB1}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45147.581418402777" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="95" xr:uid="{29F59781-2A20-324D-894E-ECA5B1C78DB1}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="10">
     <cacheField name="Tag" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="SrcTag" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Source Tag" numFmtId="0">
+    <cacheField name="SrcPort" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Source Port" numFmtId="0">
+    <cacheField name="DstTag" numFmtId="49">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="Dest Tag" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Dest Port" numFmtId="0">
+    <cacheField name="DstPort" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
-      <sharedItems containsBlank="1" count="14">
+      <sharedItems containsBlank="1" count="18">
         <s v="BMD Video"/>
         <s v="sdi"/>
-        <s v="sdi/din"/>
+        <s v="sdi_din"/>
         <s v="hdmi"/>
         <s v="Thunderbolt"/>
         <s v="usb"/>
         <s v="ndi"/>
         <s v="rtsp"/>
         <s v="viscaip"/>
+        <m/>
         <s v="cat"/>
         <s v="RGBHV"/>
-        <m/>
+        <s v="sw"/>
+        <s v="vga"/>
+        <s v="audio"/>
+        <s v="cat6e"/>
         <s v="software" u="1"/>
-        <s v="sw" u="1"/>
+        <s v="sdi/din" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Length" numFmtId="0">
@@ -863,13 +909,16 @@
     <cacheField name="Labelled?" numFmtId="0">
       <sharedItems containsBlank="1" count="4">
         <s v="na"/>
+        <s v="Yes"/>
         <s v="No"/>
-        <s v="Yes"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="Notes" numFmtId="0">
       <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="GraphFormula" numFmtId="0">
+      <sharedItems/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -881,72 +930,78 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="57">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="95">
   <r>
     <s v="2307-1800"/>
     <s v="CDMU-A001"/>
     <s v="Key"/>
     <s v="ZVIU-E004"/>
-    <s v="quad1/sdi1"/>
+    <s v="quad1_sdi1"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:Key -&gt; zviue004:quad1_sdi1 [label='2307-1800']"/>
   </r>
   <r>
     <s v="2307-1801"/>
     <s v="CDMU-A001"/>
     <s v="Fill"/>
     <s v="ZVIU-E004"/>
-    <s v="quad5/sdi2"/>
+    <s v="quad5_sdi2"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:Fill -&gt; zviue004:quad5_sdi2 [label='2307-1801']"/>
   </r>
   <r>
     <s v="2307-1802"/>
     <s v="CDMU-A001"/>
     <s v="ProjA"/>
     <s v="ZVIU-E004"/>
-    <s v="quad6/sdi4"/>
+    <s v="quad6_sdi4"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:ProjA -&gt; zviue004:quad6_sdi4 [label='2307-1802']"/>
   </r>
   <r>
     <s v="2307-1803"/>
     <s v="CDMU-A001"/>
     <s v="ProjB"/>
     <s v="ZVIU-E004"/>
-    <s v="quad7/sdi6"/>
+    <s v="quad7_sdi6"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:ProjB -&gt; zviue004:quad7_sdi6 [label='2307-1803']"/>
   </r>
   <r>
     <s v="2307-1804"/>
     <s v="CDMU-A001"/>
     <s v="ProjC"/>
     <s v="ZVIU-E004"/>
-    <s v="quad8/sdi8"/>
+    <s v="quad8_sdi8"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:ProjC -&gt; zviue004:quad8_sdi8 [label='2307-1804']"/>
   </r>
   <r>
     <s v="2307-1805"/>
     <s v="CDMU-A001"/>
     <s v="ReadDeckLink"/>
     <s v="ZVIU-E004"/>
-    <s v="quad2/sdi3"/>
+    <s v="quad2_sdi3"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="cdmua001:ReadDeckLink -&gt; zviue004:quad2_sdi3 [label='2307-1805']"/>
   </r>
   <r>
     <s v="2307-1806"/>
@@ -958,105 +1013,115 @@
     <s v="?"/>
     <x v="1"/>
     <m/>
+    <s v="zvkua003:prog -&gt; zviua005:sdi in [label='2307-1806']"/>
   </r>
   <r>
     <s v="2307-1807"/>
     <s v="ZVIU-E004"/>
-    <s v="quad3/sdi5"/>
+    <s v="quad3_sdi5"/>
     <s v="CDMU-A001"/>
     <s v="in1"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="zviue004:quad3_sdi5 -&gt; cdmua001:in1 [label='2307-1807']"/>
   </r>
   <r>
     <s v="2307-1808"/>
     <s v="ZVKU-A003"/>
-    <s v="prog"/>
+    <s v="aux"/>
     <s v="ZVIU-D001"/>
     <s v="sdi in"/>
     <x v="1"/>
     <s v="?"/>
     <x v="1"/>
     <m/>
+    <s v="zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']"/>
   </r>
   <r>
     <s v="2307-1809"/>
     <s v="ZVIU-E004"/>
-    <s v="quad4/sdi7"/>
+    <s v="quad4_sdi7"/>
     <s v="CDMU-A001"/>
     <s v="in2"/>
     <x v="0"/>
     <s v="na"/>
     <x v="0"/>
     <s v="PP7 Screen Config and BMD Desktop Video"/>
+    <s v="zviue004:quad4_sdi7 -&gt; cdmua001:in2 [label='2307-1809']"/>
   </r>
   <r>
     <s v="2307-1810"/>
     <s v="ZVIU-E004"/>
-    <s v="quad1/sdi1"/>
+    <s v="quad1_sdi1"/>
     <s v="2307-1827"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="2"/>
-    <m/>
+    <x v="1"/>
+    <m/>
+    <s v="zviue004:quad1_sdi1 -&gt; 23071827:sdi in [label='2307-1810']"/>
   </r>
   <r>
     <s v="2307-1811"/>
     <s v="ZVIU-E004"/>
-    <s v="quad5/sdi2"/>
+    <s v="quad5_sdi2"/>
     <s v="2307-1828"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="2"/>
-    <m/>
+    <x v="1"/>
+    <m/>
+    <s v="zviue004:quad5_sdi2 -&gt; 23071828:sdi in [label='2307-1811']"/>
   </r>
   <r>
     <s v="2307-1812"/>
     <s v="ZVIU-E004"/>
-    <s v="quad6/sdi4"/>
+    <s v="quad6_sdi4"/>
     <s v="ZVIU-G003"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviue004:quad6_sdi4 -&gt; zviug003:sdi in [label='2307-1812']"/>
   </r>
   <r>
     <s v="2307-1813"/>
     <s v="ZVIU-E004"/>
-    <s v="quad7/sdi6"/>
+    <s v="quad7_sdi6"/>
     <s v="ZVIU-G004"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviue004:quad7_sdi6 -&gt; zviug004:sdi in [label='2307-1813']"/>
   </r>
   <r>
     <s v="2307-1814"/>
     <s v="ZVIU-E004"/>
-    <s v="quad8/sdi8"/>
+    <s v="quad8_sdi8"/>
     <s v="ZVIU-G005"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviue004:quad8_sdi8 -&gt; zviug005:sdi in [label='2307-1814']"/>
   </r>
   <r>
     <s v="2307-1815"/>
     <s v="ZVIU-E004"/>
-    <s v="quad2/sdi3"/>
+    <s v="quad2_sdi3"/>
     <s v="ZVIU-E001"/>
     <s v="sdi in"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="2"/>
-    <m/>
+    <x v="1"/>
+    <m/>
+    <s v="zviue004:quad2_sdi3 -&gt; zviue001:sdi in [label='2307-1815']"/>
   </r>
   <r>
     <s v="2307-1816"/>
@@ -1066,8 +1131,9 @@
     <s v="in1"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviug003:hdmi -&gt; zkvua001:in1 [label='2307-1816']"/>
   </r>
   <r>
     <s v="2307-1817"/>
@@ -1077,8 +1143,9 @@
     <s v="in2"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviug004:hdmi -&gt; zkvua001:in2 [label='2307-1817']"/>
   </r>
   <r>
     <s v="2307-1818"/>
@@ -1088,8 +1155,9 @@
     <s v="in3"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviug005:hdmi -&gt; zkvua001:in3 [label='2307-1818']"/>
   </r>
   <r>
     <s v="2307-1819"/>
@@ -1099,30 +1167,33 @@
     <s v="in4"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviue001:hdmi out -&gt; zvkua001:in4 [label='2307-1819']"/>
   </r>
   <r>
     <s v="2307-1820"/>
     <s v="2307-1825"/>
     <s v="barrel"/>
     <s v="ZVIU-E004"/>
-    <s v="quad3/sdi5"/>
+    <s v="quad3_sdi5"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="23071825:barrel -&gt; zviue004:quad3_sdi5 [label='2307-1820']"/>
   </r>
   <r>
     <s v="2307-1821"/>
     <s v="2307-1826"/>
     <s v="barrel"/>
     <s v="ZVIU-E004"/>
-    <s v="quad4/sdi7"/>
+    <s v="quad4_sdi7"/>
     <x v="2"/>
     <s v="short"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="23071826:barrel -&gt; zviue004:quad4_sdi7 [label='2307-1821']"/>
   </r>
   <r>
     <s v="2307-1822"/>
@@ -1132,8 +1203,9 @@
     <s v="in2"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviua003:hdmi -&gt; zvkua003:in2 [label='2307-1822']"/>
   </r>
   <r>
     <s v="2307-1823"/>
@@ -1143,8 +1215,9 @@
     <s v="in4"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviua008:hdmi -&gt; zvkua003:in4 [label='2307-1823']"/>
   </r>
   <r>
     <s v="2307-1824"/>
@@ -1154,8 +1227,9 @@
     <s v="usbc"/>
     <x v="4"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']"/>
   </r>
   <r>
     <s v="2307-1825"/>
@@ -1165,8 +1239,9 @@
     <s v="barrel"/>
     <x v="1"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="extension of din cable via barrel connector"/>
+    <s v="zviua005:sdi -&gt; 23071820:barrel [label='2307-1825']"/>
   </r>
   <r>
     <s v="2307-1826"/>
@@ -1176,8 +1251,9 @@
     <s v="barrel"/>
     <x v="1"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="extension of din cable via barrel connector"/>
+    <s v="zviud001:sdi -&gt; 23071821:barrel [label='2307-1826']"/>
   </r>
   <r>
     <s v="2307-1827"/>
@@ -1189,6 +1265,7 @@
     <s v="?"/>
     <x v="1"/>
     <s v="extension of din cable via barrel connector"/>
+    <s v="23071810:barrel -&gt; zviua003:sdi in [label='2307-1827']"/>
   </r>
   <r>
     <s v="2307-1828"/>
@@ -1200,6 +1277,7 @@
     <s v="?"/>
     <x v="1"/>
     <s v="extension of din cable via barrel connector"/>
+    <s v="23071811:barrel -&gt; zviua008:sdi in [label='2307-1828']"/>
   </r>
   <r>
     <s v="2307-2100"/>
@@ -1209,8 +1287,9 @@
     <s v="usb"/>
     <x v="5"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviua004:usb -&gt; cumug001:usb [label='2307-2100']"/>
   </r>
   <r>
     <s v="2307-2101"/>
@@ -1220,8 +1299,9 @@
     <s v="obs"/>
     <x v="6"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="0"/>
     <s v="Need to update &quot;ndi&quot; ports with names"/>
+    <s v="cumug001:ndi -&gt; cumue001:obs [label='2307-2101']"/>
   </r>
   <r>
     <s v="2307-2102"/>
@@ -1231,8 +1311,9 @@
     <s v="obs"/>
     <x v="7"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="0"/>
     <s v="Need to update with OBS names"/>
+    <s v="camera left: -&gt; cumue001:obs [label='2307-2102']"/>
   </r>
   <r>
     <s v="2307-2103"/>
@@ -1242,8 +1323,9 @@
     <s v="obs"/>
     <x v="7"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Need to update with OBS names"/>
+    <s v="camera centre: -&gt; cumue001:obs [label='2307-2103']"/>
   </r>
   <r>
     <s v="2307-2104"/>
@@ -1253,8 +1335,9 @@
     <s v="obs"/>
     <x v="7"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Need to update with OBS names"/>
+    <s v="camera right: -&gt; cumue001:obs [label='2307-2104']"/>
   </r>
   <r>
     <s v="2307-2105"/>
@@ -1264,19 +1347,21 @@
     <s v="obs"/>
     <x v="6"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']"/>
   </r>
   <r>
     <s v="2307-2300"/>
     <s v="ZVKU-A001"/>
-    <s v="hdmi out 6"/>
+    <s v="out_6_hdmi"/>
     <s v="ZVIU-B001"/>
     <s v="hdmi in"/>
     <x v="3"/>
     <s v="?"/>
     <x v="1"/>
     <m/>
+    <s v="zvkua001:out_6_hdmi -&gt; zviub001:hdmi in [label='2307-2300']"/>
   </r>
   <r>
     <s v="2307-2301"/>
@@ -1287,10 +1372,11 @@
     <x v="3"/>
     <s v="?"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="2307-2302"/>
+    <s v="Red hdmi"/>
+    <s v="zviub001:hdmi out -&gt; zvkua003:In 1 [label='2307-2301']"/>
+  </r>
+  <r>
+    <s v="2307-2304"/>
     <s v="ZVCU-A001"/>
     <s v="sdi"/>
     <s v="ZVKU-A003"/>
@@ -1299,6 +1385,7 @@
     <s v="?"/>
     <x v="1"/>
     <m/>
+    <s v="zvcua001:sdi -&gt; zvkua003:in5 [label='2307-2304']"/>
   </r>
   <r>
     <s v="2307-2303"/>
@@ -1310,9 +1397,10 @@
     <s v="?"/>
     <x v="1"/>
     <m/>
-  </r>
-  <r>
-    <s v="2307-2304"/>
+    <s v="zvcua002:sdi -&gt; zvkua003:in6 [label='2307-2303']"/>
+  </r>
+  <r>
+    <s v="2307-2302"/>
     <s v="ZVCU-A003"/>
     <s v="sdi"/>
     <s v="ZVKU-A003"/>
@@ -1321,6 +1409,7 @@
     <s v="?"/>
     <x v="1"/>
     <m/>
+    <s v="zvcua003:sdi -&gt; zvkua003:in7 [label='2307-2302']"/>
   </r>
   <r>
     <s v="2307-2305"/>
@@ -1330,8 +1419,9 @@
     <s v="in8"/>
     <x v="1"/>
     <s v="?"/>
-    <x v="2"/>
+    <x v="1"/>
     <s v="Also labelled &quot;Y&quot;"/>
+    <s v="23072306:barrel -&gt; zvkua003:in8 [label='2307-2305']"/>
   </r>
   <r>
     <s v="2307-2306"/>
@@ -1341,8 +1431,9 @@
     <s v="barrel"/>
     <x v="1"/>
     <s v="?"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Stage Extension"/>
+    <s v="z150:sdi -&gt; 23072305:barrel [label='2307-2306']"/>
   </r>
   <r>
     <s v="2307-2307"/>
@@ -1352,8 +1443,9 @@
     <m/>
     <x v="1"/>
     <s v="?"/>
-    <x v="2"/>
+    <x v="1"/>
     <s v="unused - Also labeled &quot;C&quot; (stage to balcony)"/>
+    <s v=": -&gt; : [label='2307-2307']"/>
   </r>
   <r>
     <s v="2307-2308"/>
@@ -1365,6 +1457,7 @@
     <s v="na"/>
     <x v="0"/>
     <s v="Config is managed in the rmip10 controller"/>
+    <s v="zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']"/>
   </r>
   <r>
     <s v="2307-2309"/>
@@ -1376,6 +1469,7 @@
     <s v="na"/>
     <x v="0"/>
     <s v="Config is managed in the rmip10 controller"/>
+    <s v="zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']"/>
   </r>
   <r>
     <s v="2307-2310"/>
@@ -1385,63 +1479,69 @@
     <s v="sw"/>
     <x v="8"/>
     <s v="na"/>
-    <x v="1"/>
+    <x v="2"/>
     <s v="Config is managed in the rmip10 controller"/>
+    <s v="zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']"/>
   </r>
   <r>
     <s v="2307-2311"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v=": -&gt; : [label='2307-2311']"/>
+  </r>
+  <r>
+    <s v="2307-2312"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v=": -&gt; : [label='2307-2312']"/>
+  </r>
+  <r>
+    <s v="2307-2313"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v=": -&gt; : [label='2307-2313']"/>
+  </r>
+  <r>
+    <s v="2307-2314"/>
     <s v="ZVKU-A001"/>
-    <s v="HDbT 1"/>
-    <s v="ZVVU-A001"/>
+    <s v="out_4_HDbT"/>
+    <s v="ZVVU-0001"/>
     <s v="HDbT"/>
-    <x v="9"/>
+    <x v="10"/>
+    <s v="?"/>
+    <x v="2"/>
+    <m/>
+    <s v="zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']"/>
+  </r>
+  <r>
+    <s v="2307-2315"/>
+    <s v="ZVKU-A001"/>
+    <s v="out_7_HDbT"/>
+    <s v="ZVIU-A001"/>
+    <s v="HDbT"/>
+    <x v="10"/>
     <s v="?"/>
     <x v="1"/>
     <m/>
-  </r>
-  <r>
-    <s v="2307-2312"/>
-    <s v="ZVKU-A001"/>
-    <s v="HDbT 1"/>
-    <s v="ZVVU-A002"/>
-    <s v="HDbT"/>
-    <x v="9"/>
-    <s v="?"/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="2307-2313"/>
-    <s v="ZVKU-A001"/>
-    <s v="HDbT 1"/>
-    <s v="ZVVU-A003"/>
-    <s v="HDbT"/>
-    <x v="9"/>
-    <s v="?"/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="2307-2314"/>
-    <s v="ZVKU-A001"/>
-    <s v="HDbT 1"/>
-    <s v="ZVVU-0001"/>
-    <s v="HDbT"/>
-    <x v="9"/>
-    <s v="?"/>
-    <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="2307-2315"/>
-    <s v="ZVKU-A001"/>
-    <s v="HDbT ?"/>
-    <s v="ZVIU-A001"/>
-    <s v="HDbT"/>
-    <x v="9"/>
-    <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <s v="zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']"/>
   </r>
   <r>
     <s v="2307-2316"/>
@@ -1451,8 +1551,9 @@
     <s v="hdmi 1"/>
     <x v="3"/>
     <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <x v="2"/>
+    <m/>
+    <s v="zviua001:hdmi -&gt; zvvu0002:hdmi 1 [label='2307-2316']"/>
   </r>
   <r>
     <s v="2307-2317"/>
@@ -1460,21 +1561,23 @@
     <m/>
     <m/>
     <m/>
-    <x v="9"/>
+    <x v="10"/>
+    <s v="?"/>
+    <x v="2"/>
+    <s v="Unused category cable to lobby at TV"/>
+    <s v=": -&gt; : [label='2307-2317']"/>
+  </r>
+  <r>
+    <s v="2307-2318"/>
+    <s v="ZVKU-A001"/>
+    <s v="out_8_HDbT"/>
+    <s v="ZVIU-A002"/>
+    <s v="HDbT"/>
+    <x v="10"/>
     <s v="?"/>
     <x v="1"/>
-    <s v="Unused category cable to looby at TV"/>
-  </r>
-  <r>
-    <s v="2307-2318"/>
-    <s v="ZVKU-A001"/>
-    <s v="HDbT"/>
-    <s v="ZVIU-A002"/>
-    <s v="HDbT"/>
-    <x v="9"/>
-    <s v="?"/>
-    <x v="1"/>
-    <m/>
+    <m/>
+    <s v="zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']"/>
   </r>
   <r>
     <s v="2307-2319"/>
@@ -1484,62 +1587,526 @@
     <s v="hdmi 1"/>
     <x v="3"/>
     <s v="?"/>
+    <x v="2"/>
+    <m/>
+    <s v="zviua002:hdmi -&gt; zvvu0003:hdmi 1 [label='2307-2319']"/>
+  </r>
+  <r>
+    <s v="2307-2320"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="11"/>
+    <s v="?"/>
+    <x v="2"/>
+    <s v="Unused Balcony to Bulkhead"/>
+    <s v=": -&gt; : [label='2307-2320']"/>
+  </r>
+  <r>
+    <s v="2307-3000"/>
+    <s v="CDMU-A001"/>
+    <s v="PP_Front_SW"/>
+    <s v="hdmi_dongle"/>
+    <m/>
+    <x v="12"/>
+    <s v="na"/>
+    <x v="2"/>
+    <s v="PP7 Screen Config Front_SW to hdmi"/>
+    <s v="cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']"/>
+  </r>
+  <r>
+    <s v="2307-3001"/>
+    <s v="ZVRU-A001"/>
+    <s v="OutB"/>
+    <s v="ZVRU-A002"/>
+    <s v="sdi in"/>
     <x v="1"/>
-    <m/>
-  </r>
-  <r>
-    <s v="2307-2320"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="10"/>
+    <s v="short"/>
+    <x v="1"/>
+    <m/>
+    <s v="zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']"/>
+  </r>
+  <r>
+    <s v="2307-3002"/>
+    <s v="ZVRU-A001"/>
+    <s v="OutA"/>
+    <s v="ZVIU-A004"/>
+    <s v="sdi in"/>
+    <x v="1"/>
+    <s v="short"/>
+    <x v="1"/>
+    <m/>
+    <s v="zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']"/>
+  </r>
+  <r>
+    <s v="2307-3003"/>
+    <s v="ZVIU-A004"/>
+    <s v="hdmi out"/>
+    <s v="ZVKU-A001"/>
+    <s v="in7"/>
+    <x v="3"/>
+    <s v="medium"/>
+    <x v="1"/>
+    <m/>
+    <s v="zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']"/>
+  </r>
+  <r>
+    <s v="2307-3004"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v=": -&gt; : [label='2307-3004']"/>
+  </r>
+  <r>
+    <s v="2307-3005"/>
+    <s v="ZVKU-A003"/>
+    <s v="out5"/>
+    <s v="ZVRU-A001"/>
+    <s v="sdi in"/>
+    <x v="1"/>
     <s v="?"/>
     <x v="1"/>
-    <s v="Unused Balcony to Bulkhead"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="11"/>
-    <m/>
+    <s v="Red"/>
+    <s v="zvkua003:out5 -&gt; zvrua001:sdi in [label='2307-3005']"/>
+  </r>
+  <r>
+    <s v="2307-3006"/>
+    <s v="ZVKU-A003"/>
+    <s v="out6"/>
+    <s v="ZVIU-D002"/>
+    <s v="sdi in"/>
+    <x v="1"/>
+    <s v="?"/>
+    <x v="1"/>
+    <s v="Blue"/>
+    <s v="zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']"/>
+  </r>
+  <r>
+    <s v="2307-3007"/>
+    <s v="ZVIU-D001"/>
+    <s v="hdmi"/>
+    <s v="ZVIU-A004"/>
+    <s v="hdmi in"/>
     <x v="3"/>
-    <m/>
+    <s v="?"/>
+    <x v="1"/>
+    <m/>
+    <s v="zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']"/>
+  </r>
+  <r>
+    <s v="2308-0800"/>
+    <s v="ZVIU-A005"/>
+    <s v="hdmi"/>
+    <s v="ZVKU-A001"/>
+    <s v="in6"/>
+    <x v="3"/>
+    <s v="?"/>
+    <x v="1"/>
+    <m/>
+    <s v="zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']"/>
+  </r>
+  <r>
+    <s v="2308-0804"/>
+    <s v="2308-0802"/>
+    <s v="HdmiOut"/>
+    <s v="2308-0803"/>
+    <s v="InputD"/>
+    <x v="3"/>
+    <s v="long"/>
+    <x v="1"/>
+    <s v="Optical Hdmi"/>
+    <s v="23080802:HdmiOut -&gt; 23080803:InputD [label='2308-0804']"/>
+  </r>
+  <r>
+    <s v="2308-0805"/>
+    <s v="FrontGuest"/>
+    <m/>
+    <s v="2308-0803"/>
+    <s v="InputC"/>
+    <x v="3"/>
+    <s v="?"/>
+    <x v="1"/>
+    <s v="For guest on-stage"/>
+    <s v="frontguest: -&gt; 23080803:InputC [label='2308-0805']"/>
+  </r>
+  <r>
+    <s v="2308-0806"/>
+    <s v="CDWU-A002"/>
+    <s v="HdmiOut"/>
+    <s v="2308-0802"/>
+    <s v="in2"/>
+    <x v="3"/>
+    <s v="?"/>
+    <x v="1"/>
+    <s v="Video card HDMI Output"/>
+    <s v="cdwua002:HdmiOut -&gt; 23080802:In2 [label='2308-0806']"/>
+  </r>
+  <r>
+    <s v="2308-0807"/>
+    <s v="RearGuest"/>
+    <m/>
+    <s v="2308-0802"/>
+    <s v="in1"/>
+    <x v="3"/>
+    <s v="?"/>
+    <x v="1"/>
+    <m/>
+    <s v="rearguest: -&gt; 23080802:In1 [label='2308-0807']"/>
+  </r>
+  <r>
+    <s v="2308-0809"/>
+    <s v="CDWU-A002"/>
+    <s v="vga"/>
+    <s v="VMNU-0029"/>
+    <s v="vga"/>
+    <x v="13"/>
+    <s v="?"/>
+    <x v="2"/>
+    <m/>
+    <s v="cdwua002:vga -&gt; vmnu0029:vga [label='2308-0809']"/>
+  </r>
+  <r>
+    <s v="2308-0810"/>
+    <s v="CDWU-A002"/>
+    <s v="usb"/>
+    <s v="2308-0808"/>
+    <s v="usb"/>
+    <x v="5"/>
+    <s v="?"/>
+    <x v="2"/>
+    <m/>
+    <s v="cdwua002:usb -&gt; 23080808:usb [label='2308-0810']"/>
+  </r>
+  <r>
+    <s v="2308-0811"/>
+    <s v="rack_dev"/>
+    <m/>
+    <s v="2308-0808"/>
+    <s v="Mic_In"/>
+    <x v="14"/>
+    <s v="?"/>
+    <x v="3"/>
+    <m/>
+    <s v="rack_dev: -&gt; 23080808:Mic_In [label='2308-0811']"/>
+  </r>
+  <r>
+    <s v="2308-0900"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0900']"/>
+  </r>
+  <r>
+    <s v="2308-0901"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0901']"/>
+  </r>
+  <r>
+    <s v="2308-0902"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0902']"/>
+  </r>
+  <r>
+    <s v="2308-0903"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0903']"/>
+  </r>
+  <r>
+    <s v="2308-0904"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0904']"/>
+  </r>
+  <r>
+    <s v="2308-0905"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0905']"/>
+  </r>
+  <r>
+    <s v="2308-0906"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0906']"/>
+  </r>
+  <r>
+    <s v="2308-0907"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0907']"/>
+  </r>
+  <r>
+    <s v="2308-0908"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0908']"/>
+  </r>
+  <r>
+    <s v="2308-0909"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0909']"/>
+  </r>
+  <r>
+    <s v="2308-0910"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0910']"/>
+  </r>
+  <r>
+    <s v="2308-0911"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0911']"/>
+  </r>
+  <r>
+    <s v="2308-0912"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0912']"/>
+  </r>
+  <r>
+    <s v="2308-0913"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0913']"/>
+  </r>
+  <r>
+    <s v="2308-0914"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0914']"/>
+  </r>
+  <r>
+    <s v="2308-0915"/>
+    <s v="ZVIU-G003"/>
+    <s v="hdmi_out"/>
+    <s v="ZVKU-A001"/>
+    <s v="in1"/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']"/>
+  </r>
+  <r>
+    <s v="2308-0916"/>
+    <s v="ZVIU-G004"/>
+    <s v="hdmi_out"/>
+    <s v="ZVKU-A001"/>
+    <s v="in2"/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']"/>
+  </r>
+  <r>
+    <s v="2308-0917"/>
+    <s v="ZVIU-G005"/>
+    <s v="hdmi_out"/>
+    <s v="ZVKU-A001"/>
+    <s v="in3"/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']"/>
+  </r>
+  <r>
+    <s v="2308-0918"/>
+    <s v="2308-0919"/>
+    <s v="hdmi_out"/>
+    <s v="ZVKU-A001"/>
+    <s v="in1"/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="23080919:hdmi_out -&gt; zvkua001:in1 [label='2308-0918']"/>
+  </r>
+  <r>
+    <s v="2308-0919"/>
+    <s v="not cable"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="9"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="not cable: -&gt; : [label='2308-0919']"/>
+  </r>
+  <r>
+    <s v="PROJ0001"/>
+    <s v="ZVKU-A001"/>
+    <s v="out_1_HDbT"/>
+    <s v="ZVVU-A001"/>
+    <s v="InputD"/>
+    <x v="15"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']"/>
+  </r>
+  <r>
+    <s v="PROJ0002"/>
+    <s v="ZVKU-A001"/>
+    <s v="out_2_HDbT"/>
+    <s v="ZVVU-A002"/>
+    <s v="InputD"/>
+    <x v="15"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']"/>
+  </r>
+  <r>
+    <s v="PROJ0003"/>
+    <s v="ZVKU-A001"/>
+    <s v="out_3_HDbT"/>
+    <s v="ZVVU-A003"/>
+    <s v="InputD"/>
+    <x v="15"/>
+    <m/>
+    <x v="3"/>
+    <m/>
+    <s v="zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item x="9"/>
+      <items count="19">
+        <item x="10"/>
         <item x="3"/>
         <item x="6"/>
         <item x="7"/>
         <item x="1"/>
-        <item x="2"/>
-        <item m="1" x="12"/>
-        <item m="1" x="13"/>
+        <item m="1" x="17"/>
+        <item m="1" x="16"/>
+        <item x="12"/>
         <item x="4"/>
         <item x="5"/>
         <item x="8"/>
         <item x="0"/>
-        <item x="10"/>
         <item x="11"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1547,7 +2114,7 @@
   <rowFields count="1">
     <field x="5"/>
   </rowFields>
-  <rowItems count="13">
+  <rowItems count="17">
     <i>
       <x/>
     </i>
@@ -1564,7 +2131,7 @@
       <x v="4"/>
     </i>
     <i>
-      <x v="5"/>
+      <x v="7"/>
     </i>
     <i>
       <x v="8"/>
@@ -1583,6 +2150,18 @@
     </i>
     <i>
       <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
     </i>
     <i t="grand">
       <x/>
@@ -1607,9 +2186,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A18:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A22:B27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1620,12 +2199,13 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
         <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
@@ -1667,8 +2247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:J73" totalsRowShown="0">
-  <autoFilter ref="A1:J73" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:J81" totalsRowShown="0">
+  <autoFilter ref="A1:J81" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{6484B3DB-2BD1-7D46-B226-BA8DA8EE99F0}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{4D4529CA-209A-6349-82DA-698D5E6A0E61}" name="SrcTag" dataDxfId="1"/>
@@ -1992,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF50C43-B168-4141-91AB-135944909792}">
-  <dimension ref="A3:B23"/>
+  <dimension ref="A3:B27"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,41 +2589,41 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
+        <v>119</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5">
-        <v>10</v>
+      <c r="B5" s="7">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7">
+        <v>84</v>
+      </c>
+      <c r="B7" s="7">
         <v>3</v>
       </c>
     </row>
@@ -2051,114 +2631,152 @@
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>12</v>
+      <c r="B8" s="7">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12">
+        <v>130</v>
+      </c>
+      <c r="B12" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13">
+        <v>131</v>
+      </c>
+      <c r="B13" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14">
+        <v>143</v>
+      </c>
+      <c r="B14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="B15" s="7">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16">
-        <v>56</v>
+        <v>199</v>
+      </c>
+      <c r="B16" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>128</v>
+      <c r="A18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19">
-        <v>10</v>
+        <v>219</v>
+      </c>
+      <c r="B19" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="7">
         <v>95</v>
       </c>
-      <c r="B20">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
+      <c r="A22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="7">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2169,13 +2787,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="247" zoomScaleNormal="247" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
+      <selection pane="bottomRight" activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2195,16 +2813,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>174</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -2213,13 +2831,13 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2236,10 +2854,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -2248,7 +2866,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J33" si="0">_xlfn.CONCAT(
@@ -2277,10 +2895,10 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -2289,7 +2907,7 @@
         <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
@@ -2304,16 +2922,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -2322,7 +2940,7 @@
         <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
@@ -2337,16 +2955,16 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
@@ -2355,7 +2973,7 @@
         <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
@@ -2370,16 +2988,16 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -2388,7 +3006,7 @@
         <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
@@ -2409,10 +3027,10 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -2421,7 +3039,7 @@
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
@@ -2439,7 +3057,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
@@ -2451,7 +3069,7 @@
         <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
@@ -2466,7 +3084,7 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>26</v>
@@ -2475,7 +3093,7 @@
         <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -2484,7 +3102,7 @@
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -2499,10 +3117,10 @@
         <v>41</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>43</v>
@@ -2514,7 +3132,7 @@
         <v>34</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" t="str">
@@ -2530,7 +3148,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>26</v>
@@ -2539,7 +3157,7 @@
         <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -2548,7 +3166,7 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -2563,22 +3181,22 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -2593,22 +3211,22 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -2623,22 +3241,22 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -2653,22 +3271,22 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -2683,22 +3301,22 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -2713,22 +3331,22 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -2740,7 +3358,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -2758,7 +3376,7 @@
         <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -2770,7 +3388,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -2788,7 +3406,7 @@
         <v>34</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -2800,7 +3418,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -2818,7 +3436,7 @@
         <v>34</v>
       </c>
       <c r="H20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -2830,7 +3448,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
         <v>49</v>
@@ -2848,7 +3466,7 @@
         <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -2860,25 +3478,25 @@
         <v>23</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="F22" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -2890,25 +3508,25 @@
         <v>24</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="F23" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -2920,7 +3538,7 @@
         <v>30</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
         <v>40</v>
@@ -2938,7 +3556,7 @@
         <v>34</v>
       </c>
       <c r="H24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -2950,7 +3568,7 @@
         <v>46</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>
@@ -2968,7 +3586,7 @@
         <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -2998,7 +3616,7 @@
         <v>34</v>
       </c>
       <c r="H26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
@@ -3007,10 +3625,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>35</v>
@@ -3019,7 +3637,7 @@
         <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>35</v>
@@ -3028,10 +3646,10 @@
         <v>34</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
@@ -3040,10 +3658,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -3052,7 +3670,7 @@
         <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" t="s">
         <v>35</v>
@@ -3061,10 +3679,10 @@
         <v>34</v>
       </c>
       <c r="H28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
@@ -3073,16 +3691,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
         <v>43</v>
@@ -3094,10 +3712,10 @@
         <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
@@ -3106,16 +3724,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
@@ -3127,10 +3745,10 @@
         <v>34</v>
       </c>
       <c r="H30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
@@ -3139,28 +3757,28 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31" t="s">
         <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
@@ -3169,22 +3787,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
         <v>80</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G32" t="s">
         <v>34</v>
@@ -3193,7 +3811,7 @@
         <v>29</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
@@ -3202,19 +3820,19 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
         <v>84</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
       </c>
       <c r="G33" t="s">
         <v>34</v>
@@ -3223,7 +3841,7 @@
         <v>29</v>
       </c>
       <c r="I33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
@@ -3232,28 +3850,28 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s">
         <v>34</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" ref="J34:J65" si="1">_xlfn.CONCAT(
@@ -3270,28 +3888,28 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35" t="s">
         <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="1"/>
@@ -3300,28 +3918,28 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s">
         <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="1"/>
@@ -3330,19 +3948,19 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C37" t="s">
+        <v>223</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" t="s">
         <v>91</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" t="s">
-        <v>93</v>
       </c>
       <c r="F37" t="s">
         <v>40</v>
@@ -3351,19 +3969,19 @@
         <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:hdmi out 6 -&gt; zviub001:hdmi in [label='2307-2300']</v>
+        <v>zvkua001:out_5_hdmi -&gt; zviub001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
         <v>49</v>
@@ -3372,7 +3990,7 @@
         <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
         <v>40</v>
@@ -3381,10 +3999,10 @@
         <v>34</v>
       </c>
       <c r="H38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="1"/>
@@ -3393,10 +4011,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
         <v>35</v>
@@ -3405,7 +4023,7 @@
         <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -3414,7 +4032,7 @@
         <v>34</v>
       </c>
       <c r="H39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="1"/>
@@ -3423,10 +4041,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
@@ -3435,7 +4053,7 @@
         <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" t="s">
         <v>35</v>
@@ -3444,7 +4062,7 @@
         <v>34</v>
       </c>
       <c r="H40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="1"/>
@@ -3453,10 +4071,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
         <v>35</v>
@@ -3465,7 +4083,7 @@
         <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" t="s">
         <v>35</v>
@@ -3474,7 +4092,7 @@
         <v>34</v>
       </c>
       <c r="H41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="1"/>
@@ -3483,19 +4101,19 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F42" t="s">
         <v>35</v>
@@ -3504,10 +4122,10 @@
         <v>34</v>
       </c>
       <c r="H42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="1"/>
@@ -3516,19 +4134,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -3537,10 +4155,10 @@
         <v>34</v>
       </c>
       <c r="H43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="1"/>
@@ -3549,7 +4167,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F44" t="s">
         <v>35</v>
@@ -3558,10 +4176,10 @@
         <v>34</v>
       </c>
       <c r="H44" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" t="s">
         <v>147</v>
-      </c>
-      <c r="I44" t="s">
-        <v>149</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="1"/>
@@ -3570,22 +4188,22 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E45" t="s">
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G45" t="s">
         <v>29</v>
@@ -3594,7 +4212,7 @@
         <v>29</v>
       </c>
       <c r="I45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="1"/>
@@ -3603,22 +4221,22 @@
     </row>
     <row r="46" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C46" t="s">
         <v>28</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E46" t="s">
         <v>28</v>
       </c>
       <c r="F46" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G46" t="s">
         <v>29</v>
@@ -3627,7 +4245,7 @@
         <v>29</v>
       </c>
       <c r="I46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J46" s="5" t="str">
         <f t="shared" si="1"/>
@@ -3636,31 +4254,31 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
         <v>28</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E47" t="s">
         <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G47" t="s">
         <v>29</v>
       </c>
       <c r="H47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="1"/>
@@ -3669,169 +4287,106 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" t="s">
-        <v>177</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E48" t="s">
-        <v>119</v>
-      </c>
-      <c r="F48" t="s">
-        <v>121</v>
-      </c>
-      <c r="G48" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTa -&gt; zvvua001:HDbT [label='2307-2311']</v>
+        <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>122</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" t="s">
-        <v>178</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E49" t="s">
-        <v>119</v>
-      </c>
-      <c r="F49" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" t="s">
-        <v>34</v>
-      </c>
-      <c r="H49" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTb -&gt; zvvua002:HDbT [label='2307-2312']</v>
+        <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
-        <v>179</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E50" t="s">
-        <v>119</v>
-      </c>
-      <c r="F50" t="s">
         <v>121</v>
-      </c>
-      <c r="G50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H50" t="s">
-        <v>95</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTc -&gt; zvvua003:HDbT [label='2307-2313']</v>
+        <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E51" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" t="s">
         <v>119</v>
-      </c>
-      <c r="F51" t="s">
-        <v>121</v>
       </c>
       <c r="G51" t="s">
         <v>34</v>
       </c>
       <c r="H51" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTd -&gt; zvvu0001:HDbT [label='2307-2314']</v>
+        <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F52" t="s">
         <v>119</v>
-      </c>
-      <c r="F52" t="s">
-        <v>121</v>
       </c>
       <c r="G52" t="s">
         <v>34</v>
       </c>
       <c r="H52" t="s">
-        <v>95</v>
+        <v>222</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTe -&gt; zviua001:HDbT [label='2307-2315']</v>
+        <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="C53" t="s">
         <v>40</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F53" t="s">
         <v>40</v>
@@ -3840,7 +4395,7 @@
         <v>34</v>
       </c>
       <c r="H53" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="1"/>
@@ -3849,19 +4404,19 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F54" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G54" t="s">
         <v>34</v>
       </c>
       <c r="H54" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="1"/>
@@ -3870,49 +4425,49 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E55" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" t="s">
         <v>119</v>
-      </c>
-      <c r="F55" t="s">
-        <v>121</v>
       </c>
       <c r="G55" t="s">
         <v>34</v>
       </c>
       <c r="H55" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="1"/>
-        <v>zvkua001:HDbTf -&gt; zviua002:HDbT [label='2307-2318']</v>
+        <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
         <v>40</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F56" t="s">
         <v>40</v>
@@ -3921,7 +4476,7 @@
         <v>34</v>
       </c>
       <c r="H56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="1"/>
@@ -3930,19 +4485,19 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G57" t="s">
         <v>34</v>
       </c>
       <c r="H57" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="1"/>
@@ -3951,16 +4506,16 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F58" t="s">
         <v>28</v>
@@ -3969,10 +4524,10 @@
         <v>29</v>
       </c>
       <c r="H58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="1"/>
@@ -3981,28 +4536,28 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F59" t="s">
         <v>35</v>
       </c>
       <c r="G59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="1"/>
@@ -4011,28 +4566,28 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" t="s">
         <v>154</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C60" t="s">
-        <v>166</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E60" t="s">
-        <v>153</v>
-      </c>
-      <c r="F60" t="s">
-        <v>156</v>
-      </c>
       <c r="G60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H60" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="1"/>
@@ -4041,55 +4596,55 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" t="s">
         <v>49</v>
       </c>
+      <c r="D61" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" t="s">
+        <v>40</v>
+      </c>
       <c r="G61" t="s">
-        <v>34</v>
+        <v>205</v>
+      </c>
+      <c r="H61" t="s">
+        <v>145</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="1"/>
-        <v>zviua004:hdmi out -&gt; : [label='2307-3003']</v>
+        <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E62" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" t="s">
-        <v>40</v>
-      </c>
-      <c r="G62" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="1"/>
-        <v>: -&gt; zviua004:hdmi in [label='2307-3004']</v>
+        <v>: -&gt; : [label='2307-3004']</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E63" t="s">
         <v>43</v>
@@ -4101,10 +4656,10 @@
         <v>34</v>
       </c>
       <c r="H63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I63" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="1"/>
@@ -4113,16 +4668,16 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C64" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E64" t="s">
         <v>43</v>
@@ -4134,10 +4689,10 @@
         <v>34</v>
       </c>
       <c r="H64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I64" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="1"/>
@@ -4146,19 +4701,19 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F65" t="s">
         <v>40</v>
@@ -4167,7 +4722,7 @@
         <v>34</v>
       </c>
       <c r="H65" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="1"/>
@@ -4176,10 +4731,10 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
         <v>40</v>
@@ -4188,7 +4743,7 @@
         <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F66" t="s">
         <v>40</v>
@@ -4197,7 +4752,7 @@
         <v>34</v>
       </c>
       <c r="H66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J66" t="str">
         <f>_xlfn.CONCAT(
@@ -4214,31 +4769,31 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="C67" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
       <c r="E67" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F67" t="s">
-        <v>40</v>
+        <v>236</v>
       </c>
       <c r="G67" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I67" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="J67" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4250,21 +4805,21 @@
 " [label='",
  A67,
 "']")</f>
-        <v>23080802:HdmiOut -&gt; 23080803:InputD [label='2308-0804']</v>
+        <v>23080002:HdmiOut -&gt; 23080003:InputD [label='2308-0004']</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
       <c r="E68" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F68" t="s">
         <v>40</v>
@@ -4273,10 +4828,10 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I68" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J68" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4288,24 +4843,24 @@
 " [label='",
  A68,
 "']")</f>
-        <v>frontguest: -&gt; 23080803:InputC [label='2308-0805']</v>
+        <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C69" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="E69" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="F69" t="s">
         <v>40</v>
@@ -4314,10 +4869,10 @@
         <v>34</v>
       </c>
       <c r="H69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I69" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="J69" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4329,21 +4884,21 @@
 " [label='",
  A69,
 "']")</f>
-        <v>cdwua002:HdmiOut -&gt; 23080802:In2 [label='2308-0806']</v>
+        <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="E70" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="F70" t="s">
         <v>40</v>
@@ -4352,7 +4907,7 @@
         <v>34</v>
       </c>
       <c r="H70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J70" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4364,33 +4919,33 @@
 " [label='",
  A70,
 "']")</f>
-        <v>rearguest: -&gt; 23080802:In1 [label='2308-0807']</v>
+        <v>rearguest: -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>203</v>
+        <v>230</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E71" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F71" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="G71" t="s">
         <v>34</v>
       </c>
       <c r="H71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J71" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4402,33 +4957,33 @@
 " [label='",
  A71,
 "']")</f>
-        <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0809']</v>
+        <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="E72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G72" t="s">
         <v>34</v>
       </c>
       <c r="H72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J72" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -4440,24 +4995,24 @@
 " [label='",
  A72,
 "']")</f>
-        <v>cdwua002:usb -&gt; 23080808:usb [label='2308-0810']</v>
+        <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="E73" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="F73" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="G73" t="s">
         <v>34</v>
@@ -4472,7 +5027,257 @@
 " [label='",
  A73,
 "']")</f>
-        <v>rack_dev: -&gt; 23080808:Mic_In [label='2308-0811']</v>
+        <v>rack_dev: -&gt; 23080008:Mic_In [label='2308-0011']</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74" t="s">
+        <v>37</v>
+      </c>
+      <c r="H74" t="s">
+        <v>145</v>
+      </c>
+      <c r="J74" s="7" t="str">
+        <f t="shared" ref="J74:J77" si="2">_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B74),"-",""),
+":",  C74,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D74),"-",""),
+ ":", E74,
+" [label='",
+ A74,
+"']")</f>
+        <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C75" t="s">
+        <v>215</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="s">
+        <v>38</v>
+      </c>
+      <c r="H75" t="s">
+        <v>145</v>
+      </c>
+      <c r="J75" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>208</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C76" t="s">
+        <v>215</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" t="s">
+        <v>39</v>
+      </c>
+      <c r="H76" t="s">
+        <v>145</v>
+      </c>
+      <c r="J76" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" t="s">
+        <v>215</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" t="s">
+        <v>37</v>
+      </c>
+      <c r="H77" t="s">
+        <v>145</v>
+      </c>
+      <c r="J77" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>23080919:hdmi_out -&gt; zvkua001:in1 [label='2308-0918']</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" t="s">
+        <v>211</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E78" t="s">
+        <v>178</v>
+      </c>
+      <c r="F78" t="s">
+        <v>219</v>
+      </c>
+      <c r="H78" t="s">
+        <v>145</v>
+      </c>
+      <c r="J78" s="7" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B78),"-",""),
+":",  C78,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D78),"-",""),
+ ":", E78,
+" [label='",
+ A78,
+"']")</f>
+        <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>217</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s">
+        <v>212</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E79" t="s">
+        <v>178</v>
+      </c>
+      <c r="F79" t="s">
+        <v>219</v>
+      </c>
+      <c r="H79" t="s">
+        <v>145</v>
+      </c>
+      <c r="J79" s="7" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B79),"-",""),
+":",  C79,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D79),"-",""),
+ ":", E79,
+" [label='",
+ A79,
+"']")</f>
+        <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>218</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C80" t="s">
+        <v>213</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E80" t="s">
+        <v>178</v>
+      </c>
+      <c r="F80" t="s">
+        <v>219</v>
+      </c>
+      <c r="H80" t="s">
+        <v>145</v>
+      </c>
+      <c r="J80" s="7" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B80),"-",""),
+":",  C80,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D80),"-",""),
+ ":", E80,
+" [label='",
+ A80,
+"']")</f>
+        <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>224</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" t="s">
+        <v>223</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" t="s">
+        <v>39</v>
+      </c>
+      <c r="F81" t="s">
+        <v>40</v>
+      </c>
+      <c r="G81" t="s">
+        <v>205</v>
+      </c>
+      <c r="H81" t="s">
+        <v>145</v>
+      </c>
+      <c r="I81" t="s">
+        <v>225</v>
+      </c>
+      <c r="J81" s="7" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B81),"-",""),
+":",  C81,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D81),"-",""),
+ ":", E81,
+" [label='",
+ A81,
+"']")</f>
+        <v>zvkua001:out_5_hdmi -&gt; zvkua003:in3 [label='2308-0920']</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated diagrams and intra-doc consistency
</commit_message>
<xml_diff>
--- a/data/cables.xlsx
+++ b/data/cables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732E4573-CE94-314F-A80E-0BEE891E00CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF9AE2-987C-DE41-BF12-8221B0F08B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="760" windowWidth="24180" windowHeight="18880" activeTab="1" xr2:uid="{288904EE-D384-EA4C-9B98-052B972FB267}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="27" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="437">
   <si>
     <t>Tag</t>
   </si>
@@ -273,9 +273,6 @@
     <t>CUMU-E001</t>
   </si>
   <si>
-    <t>Need to update "ndi" ports with names</t>
-  </si>
-  <si>
     <t>camera left</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>much longer than it needs to be. 2m would been enough.</t>
+  </si>
+  <si>
+    <t>Need to update  ndi  ports with names</t>
   </si>
 </sst>
 </file>
@@ -3242,7 +3242,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C06BC8A8-0124-C241-ADED-B97F2CE891ED}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -3381,7 +3381,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{331FD294-EE6F-3D4E-A534-813A4D9D566E}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E5:F10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -3443,14 +3443,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:K135" totalsRowShown="0">
-  <autoFilter ref="A1:K135" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2308-2900"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}" name="Table1" displayName="Table1" ref="A1:K136" totalsRowShown="0">
+  <autoFilter ref="A1:K136" xr:uid="{04D71FDC-83F7-5749-A2BA-4DE157ADFDC1}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{6484B3DB-2BD1-7D46-B226-BA8DA8EE99F0}" name="Tag"/>
     <tableColumn id="2" xr3:uid="{4D4529CA-209A-6349-82DA-698D5E6A0E61}" name="SrcTag" dataDxfId="2"/>
@@ -3793,15 +3787,15 @@
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -3809,21 +3803,21 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3837,13 +3831,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7">
         <v>38</v>
@@ -3851,13 +3845,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -3865,13 +3859,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9">
         <v>53</v>
@@ -3879,13 +3873,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10">
         <v>112</v>
@@ -3901,7 +3895,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3917,7 +3911,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -3925,7 +3919,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3933,7 +3927,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -3949,7 +3943,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -3981,7 +3975,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3989,7 +3983,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -3997,7 +3991,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -4005,7 +3999,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25">
         <v>9</v>
@@ -4013,7 +4007,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26">
         <v>112</v>
@@ -4027,13 +4021,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B91ADC-4569-1C4E-B002-1ED2E647C959}">
-  <dimension ref="A1:K135"/>
+  <dimension ref="A1:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="247" zoomScaleNormal="247" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4054,16 +4048,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" t="s">
         <v>161</v>
-      </c>
-      <c r="E1" t="s">
-        <v>162</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -4072,19 +4066,19 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4098,10 +4092,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -4110,7 +4104,7 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" ref="K2:K31" si="0">_xlfn.CONCAT(
@@ -4125,7 +4119,7 @@
         <v>cdmua001:Key -&gt; zviue004:sw1 [label='2307-1800']</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4139,10 +4133,10 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
@@ -4151,14 +4145,14 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:Fill -&gt; zviue004:sw2 [label='2307-1801']</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -4172,10 +4166,10 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -4184,14 +4178,14 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:ProjA -&gt; zviue004:sw4 [label='2307-1802']</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4205,10 +4199,10 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G5" t="s">
         <v>29</v>
@@ -4217,14 +4211,14 @@
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:ProjB -&gt; zviue004:sw6 [label='2307-1803']</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4238,10 +4232,10 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -4250,14 +4244,14 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:ProjC -&gt; zviue004:sw8 [label='2307-1804']</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -4265,16 +4259,16 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -4283,32 +4277,32 @@
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:RearDeckLink -&gt; zviue004:sw3 [label='2307-1805']</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G8" t="s">
         <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
         <v>not used: -&gt; : [label='2307-1806']</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4322,10 +4316,10 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G9" t="s">
         <v>29</v>
@@ -4334,14 +4328,14 @@
         <v>29</v>
       </c>
       <c r="J9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:in1 -&gt; zviue004:sw5 [label='2307-1807']</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -4349,7 +4343,7 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>55</v>
@@ -4364,14 +4358,14 @@
         <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
         <v>zvkua003:aux -&gt; zviud001:sdi in [label='2307-1808']</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4385,10 +4379,10 @@
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F11" t="s">
         <v>387</v>
-      </c>
-      <c r="F11" t="s">
-        <v>388</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -4397,7 +4391,7 @@
         <v>29</v>
       </c>
       <c r="J11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K11" t="e">
         <f>_xlfn.CONCAT(
@@ -4412,7 +4406,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -4420,35 +4414,35 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G12" t="s">
         <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I12" t="s">
         <v>42</v>
       </c>
       <c r="J12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi1 -&gt; 23081204:sdi in [label='2307-1810']</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4456,35 +4450,35 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G13" t="s">
         <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I13" t="s">
         <v>43</v>
       </c>
       <c r="J13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi2 -&gt; 23081205:sdi in [label='2307-1811']</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4492,7 +4486,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>61</v>
@@ -4501,23 +4495,23 @@
         <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G14" t="s">
         <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi4 -&gt; zviug003:sdi in [label='2307-1812']</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -4525,7 +4519,7 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>62</v>
@@ -4534,23 +4528,23 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi6 -&gt; zviug004:sdi in [label='2307-1813']</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -4558,7 +4552,7 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>63</v>
@@ -4567,23 +4561,23 @@
         <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G16" t="s">
         <v>48</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi8 -&gt; zviug005:sdi in [label='2307-1814']</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -4591,7 +4585,7 @@
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>64</v>
@@ -4600,80 +4594,80 @@
         <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G17" t="s">
         <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
         <v>zviue004:sdi3 -&gt; zviue001:sdi in [label='2307-1815']</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
         <v>: -&gt; : [label='2307-1816']</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
         <v>: -&gt; : [label='2307-1817']</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
         <v>: -&gt; : [label='2307-1818']</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
         <v>not used: -&gt; : [label='2307-1819']</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -4687,26 +4681,26 @@
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G22" t="s">
         <v>48</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
         <v>23071825:barrel -&gt; zviue004:sdi5 [label='2307-1820']</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -4720,26 +4714,26 @@
         <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G23" t="s">
         <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
         <v>23071826:barrel -&gt; zviue004:sdi7 [label='2307-1821']</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -4753,7 +4747,7 @@
         <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F24" t="s">
         <v>39</v>
@@ -4762,14 +4756,14 @@
         <v>34</v>
       </c>
       <c r="H24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
         <v>zviua003:hdmi -&gt; zvkua003:in2_hdmi [label='2307-1822']</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -4783,7 +4777,7 @@
         <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F25" t="s">
         <v>39</v>
@@ -4792,7 +4786,7 @@
         <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I25" t="s">
         <v>43</v>
@@ -4802,7 +4796,7 @@
         <v>zviua008:hdmi -&gt; zvkua003:in4_hdmi [label='2307-1828']</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -4825,14 +4819,14 @@
         <v>34</v>
       </c>
       <c r="H26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
         <v>cdmua001:usbc -&gt; zviue005:usbc [label='2307-1824']</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>49</v>
       </c>
@@ -4855,7 +4849,7 @@
         <v>34</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>53</v>
@@ -4866,7 +4860,7 @@
         <v>zviua005:sdi -&gt; 23071820:barrel [label='2307-1825']</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -4889,7 +4883,7 @@
         <v>34</v>
       </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I28" t="s">
         <v>53</v>
@@ -4899,7 +4893,7 @@
         <v>zviud001:sdi -&gt; 23071821:barrel [label='2307-1826']</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -4913,7 +4907,7 @@
         <v>74</v>
       </c>
       <c r="E29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F29" t="s">
         <v>73</v>
@@ -4922,14 +4916,14 @@
         <v>34</v>
       </c>
       <c r="H29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
         <v>zviua004:usb -&gt; cumug001:usb_3 [label='2307-2100']</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -4943,7 +4937,7 @@
         <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
         <v>75</v>
@@ -4955,28 +4949,28 @@
         <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>77</v>
+        <v>436</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
         <v>cumug001:ndi -&gt; cumue001:obs [label='2307-2101']</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>68</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31" t="s">
         <v>34</v>
@@ -4985,37 +4979,37 @@
         <v>29</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="0"/>
         <v>camera left: -&gt; cumue001:obs [label='2307-2102']</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>69</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
         <v>34</v>
       </c>
       <c r="H32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" ref="K32:K63" si="1">_xlfn.CONCAT(
@@ -5030,37 +5024,37 @@
         <v>camera centre: -&gt; cumue001:obs [label='2307-2103']</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s">
         <v>34</v>
       </c>
       <c r="H33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="1"/>
         <v>camera right: -&gt; cumue001:obs [label='2307-2104']</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -5074,7 +5068,7 @@
         <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
         <v>75</v>
@@ -5083,28 +5077,28 @@
         <v>34</v>
       </c>
       <c r="H34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="1"/>
         <v>cdmua001:ndi -&gt; cumue001:obs [label='2307-2105']</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -5113,19 +5107,19 @@
         <v>34</v>
       </c>
       <c r="H35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
         <v>zvkua001:out_5_hdmi -&gt; zviuc001:hdmi in [label='2307-2300']</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C36" t="s">
         <v>45</v>
@@ -5134,7 +5128,7 @@
         <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F36" t="s">
         <v>39</v>
@@ -5143,22 +5137,22 @@
         <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="1"/>
         <v>zviuc001:hdmi out -&gt; zvkua003:in1_hdmi [label='2307-2301']</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>35</v>
@@ -5167,7 +5161,7 @@
         <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F37" t="s">
         <v>35</v>
@@ -5176,19 +5170,19 @@
         <v>34</v>
       </c>
       <c r="H37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="1"/>
         <v>zvcua001:sdi -&gt; zvkua003:in5_sdi [label='2307-2304']</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -5197,7 +5191,7 @@
         <v>40</v>
       </c>
       <c r="E38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F38" t="s">
         <v>35</v>
@@ -5206,19 +5200,19 @@
         <v>34</v>
       </c>
       <c r="H38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="1"/>
         <v>zvcua002:sdi -&gt; zvkua003:in6_sdi [label='2307-2303']</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
         <v>35</v>
@@ -5227,7 +5221,7 @@
         <v>40</v>
       </c>
       <c r="E39" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -5236,19 +5230,19 @@
         <v>34</v>
       </c>
       <c r="H39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="1"/>
         <v>zvcua003:sdi -&gt; zvkua003:in7_sdi [label='2307-2302']</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="C40" t="s">
         <v>65</v>
@@ -5257,7 +5251,7 @@
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F40" t="s">
         <v>35</v>
@@ -5266,28 +5260,28 @@
         <v>34</v>
       </c>
       <c r="H40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="1"/>
         <v>23072306:barrel -&gt; zvkua003:in8_sdi [label='2307-2305']</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
         <v>35</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
         <v>65</v>
@@ -5299,19 +5293,19 @@
         <v>34</v>
       </c>
       <c r="H41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="1"/>
         <v>z150:sdi -&gt; 23072305:barrel [label='2307-2306']</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
         <v>35</v>
@@ -5320,34 +5314,34 @@
         <v>34</v>
       </c>
       <c r="H42" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42" t="s">
         <v>135</v>
-      </c>
-      <c r="I42" t="s">
-        <v>136</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2307']</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
         <v>28</v>
       </c>
       <c r="F43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G43" t="s">
         <v>29</v>
@@ -5356,31 +5350,31 @@
         <v>29</v>
       </c>
       <c r="I43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="1"/>
         <v>zvkua004:sw -&gt; zvcua001:sw [label='2307-2308']</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="21" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
         <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G44" t="s">
         <v>29</v>
@@ -5389,151 +5383,151 @@
         <v>29</v>
       </c>
       <c r="I44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K44" s="5" t="str">
         <f t="shared" si="1"/>
         <v>zvkua004:sw -&gt; zvcua002:sw [label='2307-2309']</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E45" t="s">
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G45" t="s">
         <v>29</v>
       </c>
       <c r="H45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="1"/>
         <v>zvkua004:sw -&gt; zvcua003:sw [label='2307-2310']</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2311']</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2312']</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2313']</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G49" t="s">
         <v>34</v>
       </c>
       <c r="H49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="1"/>
         <v>zvkua001:out_4_HDbT -&gt; zvvu0001:HDbT [label='2307-2314']</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G50" t="s">
         <v>34</v>
       </c>
       <c r="H50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="1"/>
         <v>zvkua001:out_7_HDbT -&gt; zviua001:HDbT [label='2307-2315']</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
         <v>39</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F51" t="s">
         <v>39</v>
@@ -5542,127 +5536,127 @@
         <v>34</v>
       </c>
       <c r="H51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="1"/>
         <v>zviua001:hdmi -&gt; zvvulobby tv :hdmi 1 [label='2307-2316']</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G52" t="s">
         <v>34</v>
       </c>
       <c r="H52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2317']</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G53" t="s">
         <v>34</v>
       </c>
       <c r="H53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="1"/>
         <v>zvkua001:out_8_HDbT -&gt; zviua002:HDbT [label='2307-2318']</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="E54" t="s">
         <v>419</v>
-      </c>
-      <c r="E54" t="s">
-        <v>420</v>
       </c>
       <c r="F54" t="s">
         <v>39</v>
       </c>
       <c r="H54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="1"/>
         <v>zviua002:hdmi -&gt; 23082900:input [label='2308-3001']</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="F55" t="s">
         <v>132</v>
-      </c>
-      <c r="F55" t="s">
-        <v>133</v>
       </c>
       <c r="G55" t="s">
         <v>34</v>
       </c>
       <c r="H55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-2320']</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="F56" t="s">
         <v>28</v>
@@ -5671,31 +5665,31 @@
         <v>29</v>
       </c>
       <c r="H56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="1"/>
         <v>cdmua001:PP_Front_SW -&gt; hdmi_dongle: [label='2307-3000']</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E57" t="s">
         <v>139</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E57" t="s">
-        <v>140</v>
       </c>
       <c r="F57" t="s">
         <v>35</v>
@@ -5704,46 +5698,46 @@
         <v>48</v>
       </c>
       <c r="H57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="1"/>
         <v>zvrua001:OutB -&gt; zvrua002:SDI In [label='2307-3001']</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>140</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>72</v>
       </c>
       <c r="E58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G58" t="s">
         <v>48</v>
       </c>
       <c r="H58" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="1"/>
         <v>zvrua001:OutA -&gt; zviua004:SDI In [label='2307-3002']</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>72</v>
@@ -5755,46 +5749,46 @@
         <v>46</v>
       </c>
       <c r="E59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F59" t="s">
         <v>39</v>
       </c>
       <c r="G59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="1"/>
         <v>zviua004:hdmi out -&gt; zvkua001:in7 [label='2307-3003']</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="1"/>
         <v>: -&gt; : [label='2307-3004']</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E61" t="s">
         <v>41</v>
@@ -5806,28 +5800,28 @@
         <v>34</v>
       </c>
       <c r="H61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="1"/>
         <v>zvkua003:out5 -&gt; zvrua001:sdi in [label='2307-3005']</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
@@ -5839,19 +5833,19 @@
         <v>34</v>
       </c>
       <c r="H62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="1"/>
         <v>zvkua003:out6 -&gt; zviud002:sdi in [label='2307-3006']</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>55</v>
@@ -5863,7 +5857,7 @@
         <v>72</v>
       </c>
       <c r="E63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F63" t="s">
         <v>39</v>
@@ -5872,16 +5866,16 @@
         <v>34</v>
       </c>
       <c r="H63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="1"/>
         <v>zviud001:hdmi -&gt; zviua004:hdmi in [label='2307-3007']</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>54</v>
@@ -5893,7 +5887,7 @@
         <v>46</v>
       </c>
       <c r="E64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F64" t="s">
         <v>39</v>
@@ -5902,10 +5896,10 @@
         <v>34</v>
       </c>
       <c r="H64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I64" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" ref="K64:K71" si="2">_xlfn.CONCAT(
@@ -5920,84 +5914,84 @@
         <v>zviua005:hdmi -&gt; zvkua001:in6 [label='2308-0800']</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C65" t="s">
+      <c r="E65" t="s">
         <v>165</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="F65" t="s">
         <v>217</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>166</v>
       </c>
-      <c r="F65" t="s">
-        <v>218</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
+        <v>134</v>
+      </c>
+      <c r="I65" t="s">
         <v>167</v>
-      </c>
-      <c r="H65" t="s">
-        <v>135</v>
-      </c>
-      <c r="I65" t="s">
-        <v>168</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="2"/>
         <v>23080002:HdmiOut -&gt; 23080003:InputD [label='2308-0004']</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D66" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E66" t="s">
+        <v>168</v>
+      </c>
+      <c r="F66" t="s">
         <v>217</v>
-      </c>
-      <c r="E66" t="s">
-        <v>169</v>
-      </c>
-      <c r="F66" t="s">
-        <v>218</v>
       </c>
       <c r="G66" t="s">
         <v>34</v>
       </c>
       <c r="H66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="2"/>
         <v>frontguest: -&gt; 23080003:InputC [label='2308-0005']</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B67" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" t="s">
         <v>171</v>
-      </c>
-      <c r="C67" t="s">
-        <v>165</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="E67" t="s">
-        <v>172</v>
       </c>
       <c r="F67" t="s">
         <v>39</v>
@@ -6006,31 +6000,31 @@
         <v>34</v>
       </c>
       <c r="H67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" si="2"/>
         <v>cdwua002:HdmiOut -&gt; 23080002:In2 [label='2308-0006']</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F68" t="s">
         <v>39</v>
@@ -6039,55 +6033,55 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="2"/>
         <v>rearguest:hdmi_out -&gt; 23080002:In1 [label='2308-0007']</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E69" t="s">
         <v>178</v>
       </c>
-      <c r="E69" t="s">
-        <v>179</v>
-      </c>
       <c r="F69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G69" t="s">
         <v>34</v>
       </c>
       <c r="H69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" si="2"/>
         <v>cdwua002:vga -&gt; vmnu0029:vga [label='2308-0009']</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C70" t="s">
         <v>73</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E70" t="s">
         <v>73</v>
@@ -6099,28 +6093,28 @@
         <v>34</v>
       </c>
       <c r="H70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="2"/>
         <v>cdwua002:usb -&gt; 23080008:usb [label='2308-0010']</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>215</v>
-      </c>
       <c r="E71" t="s">
+        <v>182</v>
+      </c>
+      <c r="F71" t="s">
         <v>183</v>
-      </c>
-      <c r="F71" t="s">
-        <v>184</v>
       </c>
       <c r="G71" t="s">
         <v>34</v>
@@ -6130,15 +6124,15 @@
         <v>rack_dev: -&gt; 23080008:Mic_In [label='2308-0011']</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>46</v>
@@ -6150,10 +6144,10 @@
         <v>39</v>
       </c>
       <c r="H72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" ref="K72:K74" si="3">_xlfn.CONCAT(
@@ -6168,15 +6162,15 @@
         <v>zviug003:hdmi_out -&gt; zvkua001:in1 [label='2308-0915']</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>46</v>
@@ -6188,25 +6182,25 @@
         <v>39</v>
       </c>
       <c r="H73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I73" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="3"/>
         <v>zviug004:hdmi_out -&gt; zvkua001:in2 [label='2308-0916']</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>46</v>
@@ -6218,66 +6212,66 @@
         <v>39</v>
       </c>
       <c r="H74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I74" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="3"/>
         <v>zviug005:hdmi_out -&gt; zvkua001:in3 [label='2308-0917']</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>190</v>
+      </c>
+      <c r="B75" t="s">
         <v>191</v>
       </c>
-      <c r="B75" t="s">
-        <v>192</v>
-      </c>
       <c r="C75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E75" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F75" t="s">
         <v>39</v>
       </c>
       <c r="H75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I75" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I76" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" ref="K76:K85" si="4">_xlfn.CONCAT(
@@ -6292,81 +6286,81 @@
         <v>zvkua001:out_1_HDbT -&gt; zvvua001:InputD [label='PROJ0001']</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="4"/>
         <v>zvkua001:out_2_HDbT -&gt; zvvua002:InputD [label='PROJ0002']</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E78" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I78" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="4"/>
         <v>zvkua001:out_3_HDbT -&gt; zvvua003:InputD [label='PROJ0003']</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F79" t="s">
         <v>39</v>
       </c>
       <c r="G79" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I79" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K79" t="e">
         <f>_xlfn.CONCAT(
@@ -6381,21 +6375,21 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C80" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D80" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E80" t="s">
         <v>221</v>
-      </c>
-      <c r="E80" t="s">
-        <v>222</v>
       </c>
       <c r="F80" t="s">
         <v>73</v>
@@ -6404,25 +6398,25 @@
         <v>48</v>
       </c>
       <c r="H80" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="4"/>
         <v>cumue001:usba_2 -&gt; 23081110:usb_in [label='2308-1111']</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E81" t="s">
         <v>73</v>
@@ -6434,25 +6428,25 @@
         <v>48</v>
       </c>
       <c r="H81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="4"/>
         <v>23081110:usb_1 -&gt; 23081104:usb [label='2308-1112']</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E82" t="s">
         <v>73</v>
@@ -6464,16 +6458,16 @@
         <v>48</v>
       </c>
       <c r="H82" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="4"/>
         <v>23081110:usb_2 -&gt; 23081105:usb [label='2308-1113']</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>76</v>
@@ -6482,34 +6476,34 @@
         <v>32</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E83" t="s">
         <v>39</v>
       </c>
       <c r="F83" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G83" t="s">
         <v>48</v>
       </c>
       <c r="H83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I83" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J83" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="4"/>
         <v>cumue001:usbc -&gt; 23081106:hdmi [label='2308-1114']</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>76</v>
@@ -6518,7 +6512,7 @@
         <v>39</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E84" t="s">
         <v>39</v>
@@ -6530,28 +6524,28 @@
         <v>48</v>
       </c>
       <c r="H84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I84" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="4"/>
         <v>cumue001:hdmi -&gt; 23081107:hdmi [label='2308-1115']</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C85" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E85" t="s">
         <v>73</v>
@@ -6563,37 +6557,37 @@
         <v>48</v>
       </c>
       <c r="H85" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="4"/>
         <v>23081110:usb  -&gt; 23081103:usb [label='2308-1116']</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F86" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G86" t="s">
         <v>48</v>
       </c>
       <c r="H86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K86" t="e">
         <f>_xlfn.CONCAT(
@@ -6608,30 +6602,30 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C87" t="s">
+        <v>308</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E87" t="s">
+        <v>226</v>
+      </c>
+      <c r="F87" t="s">
         <v>228</v>
-      </c>
-      <c r="C87" t="s">
-        <v>309</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E87" t="s">
-        <v>227</v>
-      </c>
-      <c r="F87" t="s">
-        <v>229</v>
       </c>
       <c r="G87" t="s">
         <v>48</v>
       </c>
       <c r="H87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" ref="K87:K88" si="5">_xlfn.CONCAT(
@@ -6646,95 +6640,95 @@
         <v>23081100:port3 -&gt; zaiue002:ether [label='2308-1118']</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C88" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E88" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F88" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G88" t="s">
         <v>48</v>
       </c>
       <c r="H88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="5"/>
         <v>23081100:port4 -&gt; daw_guest:ether [label='2308-1119']</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>242</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C89" t="s">
+        <v>317</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E89" t="s">
+        <v>232</v>
+      </c>
+      <c r="F89" t="s">
+        <v>319</v>
+      </c>
+      <c r="G89" t="s">
+        <v>283</v>
+      </c>
+      <c r="H89" t="s">
+        <v>134</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="J89" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="K89" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>243</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B90" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C90" t="s">
         <v>318</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="D90" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E90" t="s">
         <v>233</v>
       </c>
-      <c r="F89" t="s">
-        <v>320</v>
-      </c>
-      <c r="G89" t="s">
-        <v>284</v>
-      </c>
-      <c r="H89" t="s">
-        <v>135</v>
-      </c>
-      <c r="I89" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="J89" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="K89" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>244</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="F90" t="s">
         <v>319</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E90" t="s">
-        <v>234</v>
-      </c>
-      <c r="F90" t="s">
-        <v>320</v>
-      </c>
       <c r="G90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
@@ -6751,30 +6745,30 @@
         <v>zaiue002:Ch2 -&gt; 23081102:right [label='2308-1121']</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C91" t="s">
+        <v>246</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E91" t="s">
         <v>247</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="E91" t="s">
-        <v>248</v>
       </c>
       <c r="F91" t="s">
         <v>39</v>
       </c>
       <c r="G91" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H91" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K91" t="e">
         <f>_xlfn.CONCAT(
@@ -6789,30 +6783,30 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>249</v>
+      </c>
+      <c r="B92" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="C92" t="s">
         <v>251</v>
-      </c>
-      <c r="C92" t="s">
-        <v>252</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E92" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F92" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K92" t="str">
         <f t="shared" ref="K92:K101" si="6">_xlfn.CONCAT(
@@ -6827,229 +6821,229 @@
         <v>23081124:ch1 -&gt; zvkua003:ch1_audio [label='2308-1124L']</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>253</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C93" t="s">
         <v>254</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C93" t="s">
-        <v>255</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E93" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G93" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="6"/>
         <v>23081124:ch2 -&gt; zvkua003:ch2_audio [label='2308-1124R']</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B94" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C94" t="s">
+        <v>255</v>
+      </c>
+      <c r="F94" t="s">
+        <v>183</v>
+      </c>
+      <c r="H94" t="s">
+        <v>86</v>
+      </c>
+      <c r="I94" t="s">
         <v>256</v>
-      </c>
-      <c r="F94" t="s">
-        <v>184</v>
-      </c>
-      <c r="H94" t="s">
-        <v>87</v>
-      </c>
-      <c r="I94" t="s">
-        <v>257</v>
       </c>
       <c r="K94" t="str">
         <f t="shared" si="6"/>
         <v>zakua001:aux1 -&gt; : [label='']</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B95" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C95" t="s">
+        <v>257</v>
+      </c>
+      <c r="F95" t="s">
+        <v>183</v>
+      </c>
+      <c r="H95" t="s">
+        <v>86</v>
+      </c>
+      <c r="I95" t="s">
         <v>258</v>
-      </c>
-      <c r="F95" t="s">
-        <v>184</v>
-      </c>
-      <c r="H95" t="s">
-        <v>87</v>
-      </c>
-      <c r="I95" t="s">
-        <v>259</v>
       </c>
       <c r="K95" t="str">
         <f t="shared" si="6"/>
         <v>zakua001:aux2 -&gt; : [label='']</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B96" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
+        <v>259</v>
+      </c>
+      <c r="D96" t="s">
+        <v>214</v>
+      </c>
+      <c r="E96" t="s">
+        <v>182</v>
+      </c>
+      <c r="F96" t="s">
+        <v>183</v>
+      </c>
+      <c r="H96" t="s">
+        <v>86</v>
+      </c>
+      <c r="I96" t="s">
         <v>260</v>
-      </c>
-      <c r="D96" t="s">
-        <v>215</v>
-      </c>
-      <c r="E96" t="s">
-        <v>183</v>
-      </c>
-      <c r="F96" t="s">
-        <v>184</v>
-      </c>
-      <c r="H96" t="s">
-        <v>87</v>
-      </c>
-      <c r="I96" t="s">
-        <v>261</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="6"/>
         <v>zakua001:aux4 -&gt; 23080008:Mic_In [label='']</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C97" t="s">
+        <v>267</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E97" t="s">
+        <v>262</v>
+      </c>
+      <c r="F97" t="s">
+        <v>183</v>
+      </c>
+      <c r="H97" t="s">
+        <v>86</v>
+      </c>
+      <c r="I97" t="s">
         <v>268</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E97" t="s">
-        <v>263</v>
-      </c>
-      <c r="F97" t="s">
-        <v>184</v>
-      </c>
-      <c r="H97" t="s">
-        <v>87</v>
-      </c>
-      <c r="I97" t="s">
-        <v>269</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="6"/>
         <v>23080906:out -&gt; zakua001:in12 [label='']</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B98" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C98" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E98" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F98" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="6"/>
         <v>rearguest:left -&gt; zakua001:in13 [label='']</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B99" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E99" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F99" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="6"/>
         <v>rearguest:right -&gt; zakua001:in14 [label='']</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B100" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E100" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F100" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="6"/>
         <v>cdwua002:left -&gt; zakua001:in15 [label='']</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B101" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C101" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E101" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F101" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="6"/>
         <v>cdwua002:right -&gt; zakua001:in16 [label='']</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B102" s="6" t="s">
         <v>74</v>
       </c>
@@ -7057,7 +7051,7 @@
         <v>39</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E102" t="s">
         <v>39</v>
@@ -7069,7 +7063,7 @@
         <v>48</v>
       </c>
       <c r="H102" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K102" t="e">
         <f>_xlfn.CONCAT(
@@ -7084,18 +7078,18 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B103" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E103" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F103" t="s">
         <v>73</v>
@@ -7104,7 +7098,7 @@
         <v>48</v>
       </c>
       <c r="H103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K103" t="str">
         <f>_xlfn.CONCAT(
@@ -7119,15 +7113,15 @@
         <v>cumug001:usb_2 -&gt; zviug001:usb_in [label='']</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B104" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E104" t="s">
         <v>73</v>
@@ -7139,10 +7133,10 @@
         <v>48</v>
       </c>
       <c r="H104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I104" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K104" t="str">
         <f>_xlfn.CONCAT(
@@ -7157,15 +7151,15 @@
         <v>cumug001:usb_1 -&gt; 23081202:usb [label='']</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B105" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C105" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E105" t="s">
         <v>73</v>
@@ -7177,10 +7171,10 @@
         <v>48</v>
       </c>
       <c r="H105" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I105" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K105" t="e">
         <f>_xlfn.CONCAT(
@@ -7195,30 +7189,30 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C106" t="s">
+        <v>280</v>
+      </c>
+      <c r="D106" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D106" s="6" t="s">
+      <c r="E106" t="s">
         <v>282</v>
-      </c>
-      <c r="E106" t="s">
-        <v>283</v>
       </c>
       <c r="F106" t="s">
         <v>35</v>
       </c>
       <c r="G106" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I106" t="s">
         <v>42</v>
@@ -7236,30 +7230,30 @@
         <v>23081204:sdi_out -&gt; zviue003:sdi_in [label='2307-1201']</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B107" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C107" t="s">
         <v>280</v>
-      </c>
-      <c r="C107" t="s">
-        <v>281</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E107" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F107" t="s">
         <v>35</v>
       </c>
       <c r="G107" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H107" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I107" t="s">
         <v>43</v>
@@ -7269,21 +7263,21 @@
         <v>23081205:sdi_out -&gt; zviua008:sdi_in [label='2307-1202']</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>51</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E108" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F108" t="s">
         <v>39</v>
@@ -7292,7 +7286,7 @@
         <v>34</v>
       </c>
       <c r="H108" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I108" t="s">
         <v>42</v>
@@ -7310,321 +7304,321 @@
         <v>zviue003:hdmi_out -&gt; zvkua003:in2_hdmi [label='2307-1827']</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B109" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C109" t="s">
+        <v>178</v>
+      </c>
+      <c r="D109" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="C109" t="s">
-        <v>179</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>303</v>
-      </c>
       <c r="E109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G109" t="s">
         <v>34</v>
       </c>
       <c r="H109" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K109" t="str">
         <f t="shared" si="8"/>
         <v>cdwu0009:vga -&gt; mon:vga [label='']</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>303</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C110" t="s">
+        <v>305</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E110" t="s">
         <v>304</v>
       </c>
-      <c r="B110" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="F110" t="s">
         <v>306</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="E110" t="s">
-        <v>305</v>
-      </c>
-      <c r="F110" t="s">
-        <v>307</v>
       </c>
       <c r="G110" t="s">
         <v>34</v>
       </c>
       <c r="H110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J110" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K110" t="str">
         <f t="shared" si="8"/>
         <v>prwall3:label3 -&gt; 23081100:port1 [label='2308-2001']</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>314</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C111" t="s">
         <v>315</v>
       </c>
-      <c r="B111" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C111" t="s">
-        <v>316</v>
-      </c>
       <c r="D111" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E111" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F111" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G111" t="s">
         <v>34</v>
       </c>
       <c r="H111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K111" t="str">
         <f t="shared" si="8"/>
         <v>23081102:Right -&gt; 23082003:Right [label='2308-2002']</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C112" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E112" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F112" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G112" t="s">
         <v>34</v>
       </c>
       <c r="H112" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K112" t="str">
         <f t="shared" si="8"/>
         <v>patchpanel:a -&gt; prwall3:b1 [label='a']</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>326</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C113" t="s">
         <v>327</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="D113" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="C113" t="s">
-        <v>328</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>324</v>
-      </c>
       <c r="E113" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F113" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G113" t="s">
         <v>34</v>
       </c>
       <c r="H113" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K113" t="str">
         <f t="shared" si="8"/>
         <v>modem:c -&gt; router:d [label='b']</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B114" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C114" t="s">
+        <v>330</v>
+      </c>
+      <c r="D114" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="C114" t="s">
+      <c r="E114" t="s">
         <v>331</v>
       </c>
-      <c r="D114" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="E114" t="s">
-        <v>332</v>
-      </c>
       <c r="F114" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G114" t="s">
         <v>34</v>
       </c>
       <c r="H114" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K114" t="str">
         <f t="shared" si="8"/>
         <v>router:e -&gt; nscua001:f [label='c']</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>332</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C115" t="s">
         <v>333</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="D115" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E115" t="s">
         <v>334</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E115" t="s">
-        <v>335</v>
-      </c>
       <c r="F115" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G115" t="s">
         <v>34</v>
       </c>
       <c r="H115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K115" t="str">
         <f t="shared" si="8"/>
         <v>nscua001:h -&gt; patchpanel:i [label='g']</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B116" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C116" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D116" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E116" t="s">
+        <v>331</v>
+      </c>
+      <c r="I116" t="s">
         <v>342</v>
-      </c>
-      <c r="E116" t="s">
-        <v>332</v>
-      </c>
-      <c r="I116" t="s">
-        <v>343</v>
       </c>
       <c r="K116" t="str">
         <f t="shared" si="8"/>
         <v>nscua001:a  -&gt; nscua002:f [label='']</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B117" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C117" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D117" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="E117" t="s">
+        <v>332</v>
+      </c>
+      <c r="I117" t="s">
         <v>344</v>
-      </c>
-      <c r="E117" t="s">
-        <v>333</v>
-      </c>
-      <c r="I117" t="s">
-        <v>345</v>
       </c>
       <c r="K117" t="str">
         <f t="shared" si="8"/>
         <v>nscua001:b  -&gt; nscua005:g [label='']</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B118" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C118" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E118" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K118" t="str">
         <f t="shared" si="8"/>
         <v>nscua005:c  -&gt; nscua003:h  [label='']</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B119" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C119" t="s">
+        <v>352</v>
+      </c>
+      <c r="D119" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="C119" t="s">
-        <v>353</v>
-      </c>
-      <c r="D119" s="6" t="s">
+      <c r="E119" t="s">
+        <v>334</v>
+      </c>
+      <c r="I119" t="s">
         <v>347</v>
       </c>
-      <c r="E119" t="s">
-        <v>335</v>
-      </c>
-      <c r="I119" t="s">
+      <c r="J119" t="s">
         <v>348</v>
-      </c>
-      <c r="J119" t="s">
-        <v>349</v>
       </c>
       <c r="K119" t="str">
         <f t="shared" si="8"/>
         <v>nscua003:d  -&gt; nscua004:i [label='']</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B120" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C120" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E120" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K120" t="str">
         <f t="shared" si="8"/>
         <v>nscua004:e  -&gt; 23081124:ether [label='']</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>74</v>
@@ -7633,7 +7627,7 @@
         <v>73</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E121" t="s">
         <v>32</v>
@@ -7645,7 +7639,7 @@
         <v>34</v>
       </c>
       <c r="H121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K121" t="str">
         <f t="shared" ref="K121:K131" si="9">_xlfn.CONCAT(
@@ -7660,12 +7654,12 @@
         <v>cumug001:usb -&gt; zviuc002:usbc [label='future1']</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C122" t="s">
         <v>39</v>
@@ -7674,7 +7668,7 @@
         <v>40</v>
       </c>
       <c r="E122" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F122" t="s">
         <v>39</v>
@@ -7683,52 +7677,52 @@
         <v>34</v>
       </c>
       <c r="H122" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K122" t="str">
         <f t="shared" si="9"/>
         <v>zviuc002:hdmi -&gt; zvkua003:in3_hdmi [label='future2']</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C123" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E123" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F123" t="s">
         <v>39</v>
       </c>
       <c r="G123" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K123" t="str">
         <f t="shared" si="9"/>
         <v>cdwu0009:hdmi_out -&gt; zvkua001:in5 [label='2308-2500']</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C124" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D124" t="s">
         <v>46</v>
@@ -7740,189 +7734,189 @@
         <v>39</v>
       </c>
       <c r="G124" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H124" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I124" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K124" t="str">
         <f t="shared" si="9"/>
         <v>zviue001:hdmi_out -&gt; zvkua001:in4 [label='2308-2501']</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>398</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="F125" t="s">
+        <v>306</v>
+      </c>
+      <c r="G125" t="s">
         <v>399</v>
       </c>
-      <c r="B125" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="F125" t="s">
-        <v>307</v>
-      </c>
-      <c r="G125" t="s">
+      <c r="H125" t="s">
+        <v>134</v>
+      </c>
+      <c r="I125" t="s">
         <v>400</v>
-      </c>
-      <c r="H125" t="s">
-        <v>135</v>
-      </c>
-      <c r="I125" t="s">
-        <v>401</v>
       </c>
       <c r="K125" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2502']</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>401</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="F126" t="s">
+        <v>306</v>
+      </c>
+      <c r="G126" t="s">
         <v>402</v>
       </c>
-      <c r="B126" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="F126" t="s">
-        <v>307</v>
-      </c>
-      <c r="G126" t="s">
+      <c r="H126" t="s">
+        <v>134</v>
+      </c>
+      <c r="I126" t="s">
         <v>403</v>
-      </c>
-      <c r="H126" t="s">
-        <v>135</v>
-      </c>
-      <c r="I126" t="s">
-        <v>404</v>
       </c>
       <c r="K126" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2503']</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F127" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G127" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K127" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2504']</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C128" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E128" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F128" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G128" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H128" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I128" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K128" t="str">
         <f t="shared" si="9"/>
         <v>ncsua004:portxx -&gt; cdmua001:ether [label='2308-2600']</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F129" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G129" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K129" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2700']</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F130" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G130" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K130" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2701']</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F131" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G131" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K131" t="str">
         <f t="shared" si="9"/>
         <v>not used: -&gt; : [label='2308-2702']</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G132" t="s">
+        <v>422</v>
+      </c>
+      <c r="J132" t="s">
         <v>423</v>
       </c>
-      <c r="J132" t="s">
-        <v>424</v>
-      </c>
-      <c r="K132" s="10" t="e">
+      <c r="K132" t="e">
         <f>_xlfn.CONCAT(
 SUBSTITUTE(LOWER(#REF!),"-",""),
 ":",  C134,
@@ -7940,30 +7934,30 @@
         <v>22</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C133" t="s">
+        <v>424</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E133" t="s">
         <v>425</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E133" t="s">
-        <v>426</v>
       </c>
       <c r="F133" t="s">
         <v>39</v>
       </c>
       <c r="G133" t="s">
+        <v>434</v>
+      </c>
+      <c r="H133" t="s">
+        <v>134</v>
+      </c>
+      <c r="J133" t="s">
         <v>435</v>
       </c>
-      <c r="H133" t="s">
-        <v>135</v>
-      </c>
-      <c r="J133" t="s">
-        <v>436</v>
-      </c>
-      <c r="K133" s="10" t="str">
+      <c r="K133" t="str">
         <f>_xlfn.CONCAT(
 SUBSTITUTE(LOWER(B133),"-",""),
 ":",  C133,
@@ -7978,19 +7972,19 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C134" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D134" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E134" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F134" t="s">
         <v>39</v>
@@ -7999,9 +7993,9 @@
         <v>48</v>
       </c>
       <c r="H134" t="s">
-        <v>135</v>
-      </c>
-      <c r="K134" s="10" t="e">
+        <v>134</v>
+      </c>
+      <c r="K134" t="e">
         <f>_xlfn.CONCAT(
 SUBSTITUTE(LOWER(#REF!),"-",""),
 ":",#REF!,
@@ -8014,32 +8008,32 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C135" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D135" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="E135" t="s">
         <v>431</v>
       </c>
-      <c r="E135" t="s">
-        <v>432</v>
-      </c>
       <c r="F135" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G135" t="s">
         <v>34</v>
       </c>
       <c r="H135" t="s">
-        <v>87</v>
-      </c>
-      <c r="K135" s="10" t="str">
+        <v>86</v>
+      </c>
+      <c r="K135" t="str">
         <f>_xlfn.CONCAT(
 SUBSTITUTE(LOWER(B135),"-",""),
 ":",  C135,
@@ -8052,6 +8046,23 @@
         <v>zvkua001:out6 -&gt; unknown:unk [label='future135']</v>
       </c>
     </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E136" t="s">
+        <v>431</v>
+      </c>
+      <c r="K136" s="10" t="str">
+        <f>_xlfn.CONCAT(
+SUBSTITUTE(LOWER(B136),"-",""),
+":",  C136,
+ " -&gt; ",
+SUBSTITUTE(LOWER(D136),"-",""),
+ ":", E136,
+" [label='",
+ A136,
+"']")</f>
+        <v>: -&gt; :unk [label='']</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>